<commit_message>
fill ssl result in xlsx
</commit_message>
<xml_diff>
--- a/TrainDetail.xlsx
+++ b/TrainDetail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FengHZ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\projects\mixupfamily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A935FA24-A12E-41D8-A00B-93F9FEACAE62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A57B0BA-0F4E-4FF6-82BC-E1F2AD0F874E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,9 +289,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -333,6 +330,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,7 +617,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -640,63 +640,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="E1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -705,25 +705,25 @@
       <c r="F3" s="1">
         <v>0.2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>0.94669999999999999</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>0.99229999999999996</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -731,10 +731,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="E4" s="1">
@@ -743,7 +743,7 @@
       <c r="F4" s="1">
         <v>0.1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1E-4</v>
       </c>
       <c r="H4" s="1">
@@ -755,7 +755,7 @@
       <c r="J4" s="1">
         <v>0.2</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>0.9516</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -763,10 +763,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -775,7 +775,7 @@
       <c r="F5" s="1">
         <v>0.2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>1E-4</v>
       </c>
       <c r="H5" s="1">
@@ -787,7 +787,7 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>0.95579999999999998</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -795,12 +795,12 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -809,25 +809,25 @@
       <c r="F6" s="1">
         <v>0.2</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H6" s="1">
         <v>0.3</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>0.95920000000000005</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>0.99809999999999999</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -835,10 +835,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="2">
         <v>5</v>
       </c>
       <c r="E7" s="1">
@@ -847,51 +847,51 @@
       <c r="F7" s="1">
         <v>0.2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>1E-4</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="1">
         <v>0.2</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>0.9617</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="7">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7">
         <v>0.2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>1E-4</v>
       </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>4</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>0.97160000000000002</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -899,10 +899,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="2">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -911,7 +911,7 @@
       <c r="F9" s="1">
         <v>0.2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>1E-4</v>
       </c>
       <c r="H9" s="1">
@@ -923,7 +923,7 @@
       <c r="J9" s="1">
         <v>4</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>0.96509999999999996</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -931,10 +931,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="2">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -943,7 +943,7 @@
       <c r="F10" s="1">
         <v>0.2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>1E-4</v>
       </c>
       <c r="H10" s="1">
@@ -955,7 +955,7 @@
       <c r="J10" s="1">
         <v>4</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>0.96919999999999995</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -963,14 +963,14 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="17">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -979,7 +979,7 @@
       <c r="F11" s="1">
         <v>0.1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H11" s="1">
@@ -991,13 +991,13 @@
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>0.95150000000000001</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>0.97929999999999995</v>
       </c>
       <c r="N11" s="1" t="s">
@@ -1005,10 +1005,10 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="2">
         <v>10</v>
       </c>
       <c r="E12" s="1">
@@ -1017,7 +1017,7 @@
       <c r="F12" s="1">
         <v>0.1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>1E-4</v>
       </c>
       <c r="H12" s="1">
@@ -1029,7 +1029,7 @@
       <c r="J12" s="1">
         <v>0.2</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>0.95789999999999997</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -1037,10 +1037,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="2">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1049,7 +1049,7 @@
       <c r="F13" s="1">
         <v>0.2</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>1E-4</v>
       </c>
       <c r="H13" s="1">
@@ -1061,7 +1061,7 @@
       <c r="J13" s="1">
         <v>2</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>0.96450000000000002</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1069,12 +1069,12 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17">
         <v>34</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1083,22 +1083,22 @@
       <c r="F14" s="1">
         <v>0.1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H14" s="1">
         <v>0.3</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>0.9546</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="15" t="s">
         <v>40</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -1106,10 +1106,10 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="2">
         <v>13</v>
       </c>
       <c r="E15" s="1">
@@ -1118,7 +1118,7 @@
       <c r="F15" s="1">
         <v>0.1</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>1E-4</v>
       </c>
       <c r="H15" s="1">
@@ -1130,7 +1130,7 @@
       <c r="J15" s="1">
         <v>0.2</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>0.95540000000000003</v>
       </c>
       <c r="N15" s="1" t="s">
@@ -1138,10 +1138,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="2">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1150,7 +1150,7 @@
       <c r="F16" s="1">
         <v>0.2</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>1E-4</v>
       </c>
       <c r="H16" s="1">
@@ -1167,12 +1167,12 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17">
         <v>152</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1181,19 +1181,19 @@
       <c r="F17" s="1">
         <v>0.2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H17" s="1">
         <v>0.3</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>0.95499999999999996</v>
       </c>
       <c r="N17" s="1" t="s">
@@ -1201,10 +1201,10 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="2">
         <v>16</v>
       </c>
       <c r="E18" s="1">
@@ -1212,10 +1212,10 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="2">
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1223,14 +1223,14 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="17">
         <v>121</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1239,19 +1239,19 @@
       <c r="F20" s="1">
         <v>0.2</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H20" s="1">
         <v>0.3</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>0.95599999999999996</v>
       </c>
       <c r="N20" s="1" t="s">
@@ -1259,10 +1259,10 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="2">
         <v>19</v>
       </c>
       <c r="E21" s="1">
@@ -1271,7 +1271,7 @@
       <c r="F21" s="1">
         <v>0.1</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>1E-4</v>
       </c>
       <c r="H21" s="1">
@@ -1283,7 +1283,7 @@
       <c r="J21" s="1">
         <v>0.2</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>0.95840000000000003</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -1291,44 +1291,44 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="2">
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+    <row r="23" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <v>21</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="12">
+      <c r="E23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="11">
         <v>0.2</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <v>0.3</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="15">
+      <c r="J23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="14">
         <v>0.93710000000000004</v>
       </c>
       <c r="N23" s="1" t="s">
@@ -1336,10 +1336,10 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="2">
         <v>22</v>
       </c>
       <c r="E24" s="1">
@@ -1347,10 +1347,10 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="2">
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1358,34 +1358,34 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="D27" s="3"/>
-      <c r="J27" s="3" t="s">
+      <c r="D27" s="2"/>
+      <c r="J27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="M27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>1</v>
       </c>
       <c r="E28" s="1">
@@ -1394,7 +1394,7 @@
       <c r="F28" s="1">
         <v>0.2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H28" s="1">
@@ -1414,10 +1414,10 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -1426,7 +1426,7 @@
       <c r="F29" s="1">
         <v>0.2</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H29" s="1">
@@ -1443,12 +1443,12 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="1">
@@ -1457,7 +1457,7 @@
       <c r="F30" s="1">
         <v>0.2</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H30" s="1">
@@ -1469,15 +1469,18 @@
       <c r="J30" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="K30" s="1">
+        <v>93.06</v>
+      </c>
       <c r="N30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="2">
         <v>4</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -1486,13 +1489,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="A3:A25"/>
@@ -1503,6 +1499,13 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1533,274 +1536,274 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0.94669999999999999</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.99229999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>0.9516</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>0.95579999999999998</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.95920000000000005</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0.99809999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="2">
         <v>5</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0.9617</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="7">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="9">
         <v>0.97160000000000002</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="2">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>0.96509999999999996</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="2">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>0.96919999999999995</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="17">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>0.95150000000000001</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.97929999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="2">
         <v>10</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>0.95789999999999997</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="2">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>0.96450000000000002</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17">
         <v>34</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>0.9546</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>40</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="2">
         <v>13</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>0.95540000000000003</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="2">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1811,28 +1814,28 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17">
         <v>152</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>0.95499999999999996</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="2">
         <v>16</v>
       </c>
       <c r="E18" s="1">
@@ -1843,10 +1846,10 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="2">
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1857,46 +1860,46 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="17">
         <v>121</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>0.95599999999999996</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="2">
         <v>19</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>0.95840000000000003</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="2">
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1907,28 +1910,28 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <v>21</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="15">
+      <c r="E23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="14">
         <v>0.93710000000000004</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="2">
         <v>22</v>
       </c>
       <c r="E24" s="1">
@@ -1939,10 +1942,10 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="2">
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1956,29 +1959,29 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="1">
@@ -1991,10 +1994,10 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="2">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -2005,12 +2008,12 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>3</v>
       </c>
       <c r="E29" s="1">
@@ -2021,10 +2024,10 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="2">
         <v>4</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -2036,13 +2039,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A3:A25"/>
     <mergeCell ref="B3:B10"/>
@@ -2052,6 +2048,13 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
"modify wrn, preactres error"
</commit_message>
<xml_diff>
--- a/TrainDetail.xlsx
+++ b/TrainDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\projects\mixupfamily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80E1D6-B467-4CBD-A0F5-A315D64B9338}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91B69E4-1930-493F-85DA-778550EF3E18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Detail" sheetId="1" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>76.54% | 93.26%</t>
   </si>
   <si>
-    <t>python main_sl.py -t 1 --depth 28 --width 2  --dataset dataset -bp basepath</t>
-  </si>
-  <si>
     <t>python main_sl.py -t 9 --net-name "preactres18"  --dataset dataset -bp basepath -ad [100,150] --lr-decay-ratio 0.1</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>[150,300,450]/[80,150,190](SVHN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -736,7 +736,7 @@
         <v>0.96250000000000002</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -768,7 +768,7 @@
         <v>0.9516</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
@@ -800,7 +800,7 @@
         <v>0.95579999999999998</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
@@ -825,7 +825,7 @@
         <v>0.3</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
@@ -840,7 +840,7 @@
         <v>0.96660000000000001</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
@@ -872,7 +872,7 @@
         <v>0.9617</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.45">
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="7">
         <v>4</v>
@@ -907,7 +907,7 @@
         <v>0.97070000000000001</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
@@ -939,7 +939,7 @@
         <v>0.96509999999999996</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
@@ -971,7 +971,7 @@
         <v>0.96919999999999995</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
@@ -1043,7 +1043,7 @@
         <v>0.95789999999999997</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
@@ -1075,7 +1075,7 @@
         <v>0.96450000000000002</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
@@ -1112,7 +1112,7 @@
         <v>40</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
@@ -1144,7 +1144,7 @@
         <v>0.95540000000000003</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -1173,7 +1173,7 @@
         <v>4</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
@@ -1207,7 +1207,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.45">
@@ -1265,7 +1265,7 @@
         <v>0.95599999999999996</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.45">
@@ -1297,7 +1297,7 @@
         <v>0.95840000000000003</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
@@ -1342,7 +1342,7 @@
         <v>0.93710000000000004</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
@@ -1520,11 +1520,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="A3:A25"/>
     <mergeCell ref="B3:B10"/>
@@ -1537,6 +1532,11 @@
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix the ssl part result, add another function for mixup method
</commit_message>
<xml_diff>
--- a/TrainDetail.xlsx
+++ b/TrainDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\projects\mixupfamily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91B69E4-1930-493F-85DA-778550EF3E18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC283A39-F321-4EED-A226-D5B8C3A6EA3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Detail" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>BC190</t>
   </si>
   <si>
-    <t>Mixup Alpha(u/s)</t>
-  </si>
-  <si>
     <t>400 Labeled Per Class</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Mixup Alpha(s/u)</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>15</v>
@@ -730,13 +730,13 @@
         <v>0.94669999999999999</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" s="5">
         <v>0.96250000000000002</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -768,7 +768,7 @@
         <v>0.9516</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" s="1">
         <v>4</v>
@@ -800,7 +800,7 @@
         <v>0.95579999999999998</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
@@ -825,7 +825,7 @@
         <v>0.3</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
@@ -834,13 +834,13 @@
         <v>0.95920000000000005</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" s="5">
         <v>0.96660000000000001</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
@@ -872,7 +872,7 @@
         <v>0.9617</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.45">
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="7">
         <v>4</v>
@@ -907,7 +907,7 @@
         <v>0.97070000000000001</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
@@ -918,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1">
         <v>0.2</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="1">
         <v>4</v>
@@ -939,7 +939,7 @@
         <v>0.96509999999999996</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
@@ -950,7 +950,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1">
         <v>0.2</v>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" s="1">
         <v>4</v>
@@ -971,7 +971,7 @@
         <v>0.96919999999999995</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
@@ -1007,11 +1007,11 @@
         <v>0.95150000000000001</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
@@ -1043,7 +1043,7 @@
         <v>0.95789999999999997</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="1">
         <v>2</v>
@@ -1075,7 +1075,7 @@
         <v>0.96450000000000002</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
@@ -1109,10 +1109,10 @@
         <v>0.9546</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
@@ -1144,7 +1144,7 @@
         <v>0.95540000000000003</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -1167,13 +1167,13 @@
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J16" s="1">
         <v>4</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
@@ -1207,7 +1207,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.45">
@@ -1265,7 +1265,7 @@
         <v>0.95599999999999996</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.45">
@@ -1297,7 +1297,7 @@
         <v>0.95840000000000003</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
@@ -1342,7 +1342,7 @@
         <v>0.93710000000000004</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
@@ -1373,21 +1373,21 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D27" s="2"/>
       <c r="J27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>13</v>
@@ -1411,16 +1411,16 @@
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K28" s="1">
-        <v>90.74</v>
+        <v>93.22</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.45">
@@ -1443,16 +1443,16 @@
         <v>0</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" s="1">
         <v>89.66</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.45">
@@ -1477,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K30" s="1">
-        <v>93.06</v>
+        <v>96.22</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.45">
@@ -1509,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K31" s="1">
         <v>90.23</v>
@@ -1614,7 +1614,7 @@
         <v>0.94669999999999999</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -1666,7 +1666,7 @@
         <v>0.95920000000000005</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -1710,7 +1710,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="5">
         <v>0.96509999999999996</v>
@@ -1726,7 +1726,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="5">
         <v>0.96919999999999995</v>
@@ -1752,7 +1752,7 @@
         <v>0.95150000000000001</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="5"/>
     </row>
@@ -1804,7 +1804,7 @@
         <v>0.9546</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1987,18 +1987,18 @@
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>13</v>

</xml_diff>